<commit_message>
build: Add OOP code version.
</commit_message>
<xml_diff>
--- a/Elevation_data.xlsx
+++ b/Elevation_data.xlsx
@@ -3,90 +3,93 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="60" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
+      <charset val="238"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
       <name val="Calibri"/>
       <charset val="238"/>
       <family val="2"/>
       <b val="1"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <charset val="238"/>
+      <family val="2"/>
       <b val="1"/>
-      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill/>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom>
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin"/>
@@ -96,23 +99,23 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -187,9 +190,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -197,10 +200,10 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="EEECE1"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="1F497D"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="4F81BD"/>
@@ -227,79 +230,19 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="SimSun"/>
+        <a:cs typeface="Times New Roman"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,7 +409,36 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr>
+        <a:prstTxWarp prst="textNoShape">
+          <a:avLst/>
+        </a:prstTxWarp>
+        <a:noAutofit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr>
+          <a:defRPr/>
+        </a:defPPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
@@ -479,18 +451,18 @@
   </sheetPr>
   <dimension ref="A1:F164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.4"/>
   <cols>
-    <col width="13.1796875" customWidth="1" min="1" max="1"/>
-    <col width="14.54296875" customWidth="1" min="2" max="2"/>
-    <col width="18.1796875" customWidth="1" min="3" max="3"/>
-    <col width="18.90625" customWidth="1" min="4" max="4"/>
-    <col width="16.7265625" customWidth="1" min="5" max="5"/>
-    <col width="20.453125" customWidth="1" min="6" max="6"/>
+    <col width="13.178571" customWidth="1" min="1" max="1"/>
+    <col width="14.544643" customWidth="1" min="2" max="2"/>
+    <col width="18.178571" customWidth="1" min="3" max="3"/>
+    <col width="18.901786" customWidth="1" min="4" max="4"/>
+    <col width="16.723214" customWidth="1" min="5" max="5"/>
+    <col width="20.455357" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -506,22 +478,22 @@
       </c>
       <c r="C1" s="4" t="inlineStr">
         <is>
-          <t>Nowe odc. [m]</t>
+          <t>New dist. [m]</t>
         </is>
       </c>
       <c r="D1" s="4" t="inlineStr">
         <is>
-          <t>Delta odc. [m]</t>
+          <t>Dist. delta [m]</t>
         </is>
       </c>
       <c r="E1" s="4" t="inlineStr">
         <is>
-          <t>Nowe wys. [m]</t>
+          <t>New height [m]</t>
         </is>
       </c>
       <c r="F1" s="4" t="inlineStr">
         <is>
-          <t>Delta wys. [m]</t>
+          <t>Height delta [m]</t>
         </is>
       </c>
     </row>
@@ -539,7 +511,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>95.70407601900855</v>
+        <v>95.70393130616552</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -559,7 +531,7 @@
         <v>1710.98</v>
       </c>
       <c r="E3" t="n">
-        <v>92.29799892597573</v>
+        <v>92.29800324410687</v>
       </c>
       <c r="F3" t="n">
         <v>-3.41</v>
@@ -579,7 +551,7 @@
         <v>1710.98</v>
       </c>
       <c r="E4" t="n">
-        <v>94.38955281470223</v>
+        <v>94.38960880800826</v>
       </c>
       <c r="F4" t="n">
         <v>2.09</v>
@@ -599,7 +571,7 @@
         <v>1710.98</v>
       </c>
       <c r="E5" t="n">
-        <v>98.97794516449923</v>
+        <v>98.97800152758366</v>
       </c>
       <c r="F5" t="n">
         <v>4.59</v>
@@ -619,7 +591,7 @@
         <v>1710.98</v>
       </c>
       <c r="E6" t="n">
-        <v>104.1742673182054</v>
+        <v>104.1743027420489</v>
       </c>
       <c r="F6" t="n">
         <v>5.2</v>
@@ -639,7 +611,7 @@
         <v>1710.98</v>
       </c>
       <c r="E7" t="n">
-        <v>108.9132437579272</v>
+        <v>108.9132548679863</v>
       </c>
       <c r="F7" t="n">
         <v>4.74</v>
@@ -659,7 +631,7 @@
         <v>1710.98</v>
       </c>
       <c r="E8" t="n">
-        <v>112.7129422530651</v>
+        <v>112.7129348968484</v>
       </c>
       <c r="F8" t="n">
         <v>3.8</v>
@@ -679,7 +651,7 @@
         <v>1710.98</v>
       </c>
       <c r="E9" t="n">
-        <v>115.4785325389194</v>
+        <v>115.4785158313862</v>
       </c>
       <c r="F9" t="n">
         <v>2.77</v>
@@ -699,7 +671,7 @@
         <v>1710.98</v>
       </c>
       <c r="E10" t="n">
-        <v>117.3461811841728</v>
+        <v>117.3461637702878</v>
       </c>
       <c r="F10" t="n">
         <v>1.87</v>
@@ -719,7 +691,7 @@
         <v>1710.98</v>
       </c>
       <c r="E11" t="n">
-        <v>118.5631703055444</v>
+        <v>118.563158350314</v>
       </c>
       <c r="F11" t="n">
         <v>1.22</v>
@@ -739,7 +711,7 @@
         <v>1710.98</v>
       </c>
       <c r="E12" t="n">
-        <v>119.4003277879091</v>
+        <v>119.4003242552161</v>
       </c>
       <c r="F12" t="n">
         <v>0.84</v>
@@ -759,7 +731,7 @@
         <v>1710.98</v>
       </c>
       <c r="E13" t="n">
-        <v>120.0928566681798</v>
+        <v>120.0928615007231</v>
       </c>
       <c r="F13" t="n">
         <v>0.6899999999999999</v>
@@ -779,7 +751,7 @@
         <v>1710.98</v>
       </c>
       <c r="E14" t="n">
-        <v>120.8056513412459</v>
+        <v>120.8056622048817</v>
       </c>
       <c r="F14" t="n">
         <v>0.71</v>
@@ -799,7 +771,7 @@
         <v>1710.98</v>
       </c>
       <c r="E15" t="n">
-        <v>121.6191882462662</v>
+        <v>121.6192015530385</v>
       </c>
       <c r="F15" t="n">
         <v>0.8100000000000001</v>
@@ -819,7 +791,7 @@
         <v>1710.98</v>
       </c>
       <c r="E16" t="n">
-        <v>122.5320786916071</v>
+        <v>122.5320906667475</v>
       </c>
       <c r="F16" t="n">
         <v>0.91</v>
@@ -839,7 +811,7 @@
         <v>1710.98</v>
       </c>
       <c r="E17" t="n">
-        <v>123.4763714767231</v>
+        <v>123.4763790858901</v>
       </c>
       <c r="F17" t="n">
         <v>0.9399999999999999</v>
@@ -859,7 +831,7 @@
         <v>1710.98</v>
       </c>
       <c r="E18" t="n">
-        <v>124.3416929692791</v>
+        <v>124.3416945732932</v>
       </c>
       <c r="F18" t="n">
         <v>0.87</v>
@@ -879,7 +851,7 @@
         <v>1710.98</v>
       </c>
       <c r="E19" t="n">
-        <v>125.0043122958063</v>
+        <v>125.0043079511323</v>
       </c>
       <c r="F19" t="n">
         <v>0.66</v>
@@ -899,7 +871,7 @@
         <v>1710.98</v>
       </c>
       <c r="E20" t="n">
-        <v>125.357219304176</v>
+        <v>125.3572106784061</v>
       </c>
       <c r="F20" t="n">
         <v>0.35</v>
@@ -919,7 +891,7 @@
         <v>1710.98</v>
       </c>
       <c r="E21" t="n">
-        <v>125.3373029562212</v>
+        <v>125.3372928787584</v>
       </c>
       <c r="F21" t="n">
         <v>-0.02</v>
@@ -939,7 +911,7 @@
         <v>1710.98</v>
       </c>
       <c r="E22" t="n">
-        <v>124.9457178087492</v>
+        <v>124.94570952796</v>
       </c>
       <c r="F22" t="n">
         <v>-0.39</v>
@@ -959,7 +931,7 @@
         <v>1710.98</v>
       </c>
       <c r="E23" t="n">
-        <v>124.2575262412838</v>
+        <v>124.2575225102969</v>
       </c>
       <c r="F23" t="n">
         <v>-0.6899999999999999</v>
@@ -979,7 +951,7 @@
         <v>1710.98</v>
       </c>
       <c r="E24" t="n">
-        <v>123.4167040888344</v>
+        <v>123.4167062531906</v>
       </c>
       <c r="F24" t="n">
         <v>-0.84</v>
@@ -999,7 +971,7 @@
         <v>1710.98</v>
       </c>
       <c r="E25" t="n">
-        <v>122.6125973379158</v>
+        <v>122.6126046493085</v>
       </c>
       <c r="F25" t="n">
         <v>-0.8</v>
@@ -1019,7 +991,7 @@
         <v>1710.98</v>
       </c>
       <c r="E26" t="n">
-        <v>122.0339175442509</v>
+        <v>122.0339269754647</v>
       </c>
       <c r="F26" t="n">
         <v>-0.58</v>
@@ -1039,7 +1011,7 @@
         <v>1710.98</v>
       </c>
       <c r="E27" t="n">
-        <v>121.7963636302875</v>
+        <v>121.7963705175853</v>
       </c>
       <c r="F27" t="n">
         <v>-0.24</v>
@@ -1059,7 +1031,7 @@
         <v>1710.98</v>
       </c>
       <c r="E28" t="n">
-        <v>121.8399577209493</v>
+        <v>121.8399576110378</v>
       </c>
       <c r="F28" t="n">
         <v>0.04</v>
@@ -1079,7 +1051,7 @@
         <v>1710.98</v>
       </c>
       <c r="E29" t="n">
-        <v>121.7921826758884</v>
+        <v>121.7921748056206</v>
       </c>
       <c r="F29" t="n">
         <v>-0.05</v>
@@ -1099,7 +1071,7 @@
         <v>1710.98</v>
       </c>
       <c r="E30" t="n">
-        <v>120.7930089764704</v>
+        <v>120.7930018644279</v>
       </c>
       <c r="F30" t="n">
         <v>-1</v>
@@ -1119,7 +1091,7 @@
         <v>1710.98</v>
       </c>
       <c r="E31" t="n">
-        <v>117.2778986258636</v>
+        <v>117.277918306015</v>
       </c>
       <c r="F31" t="n">
         <v>-3.52</v>
@@ -2191,6 +2163,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" fitToHeight="1" fitToWidth="0"/>
 </worksheet>
 </file>
</xml_diff>